<commit_message>
Update spreadsheet to latest version
</commit_message>
<xml_diff>
--- a/__digital_preservation_transfer.xlsx
+++ b/__digital_preservation_transfer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/payten/Development/qsa/dps/digipres_test_corpus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D81DF7-DF07-014D-AF29-22394E43E3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D616E31-9991-0148-B505-393AD8A77276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="36300" windowHeight="18520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="449">
   <si>
     <t>Required</t>
   </si>
@@ -1357,19 +1357,22 @@
     <t>Volume/register - Spiral bound</t>
   </si>
   <si>
-    <t>Record Type to Create (ITM, DIGITAL_OBJECT)</t>
-  </si>
-  <si>
-    <t>Optional (DIGITAL_OBJECT only)</t>
-  </si>
-  <si>
-    <t>Create DRs on Parent?</t>
-  </si>
-  <si>
-    <t>Required (DIGITAL_OBJECT only)</t>
-  </si>
-  <si>
-    <t>DIGITAL_OBJECT</t>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>DR_ATTACH</t>
+  </si>
+  <si>
+    <t>Optional (ITM, DO)</t>
+  </si>
+  <si>
+    <t>Required (ITM, DO)</t>
+  </si>
+  <si>
+    <t>Required (DO, DR_ATTACH)</t>
+  </si>
+  <si>
+    <t>Record Type to Create (ITM, DO, DR_ATTACH)</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1383,7 @@
     <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1448,12 +1451,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1496,7 +1493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1548,7 +1545,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1717,7 +1713,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="RecordType" displayName="RecordType" ref="A2:A3" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="RecordType" displayName="RecordType" ref="A2:A4" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="ITM"/>
   </tableColumns>
@@ -2031,37 +2027,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1038"/>
+  <dimension ref="A1:S1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="40" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="39" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="32.1640625" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" customWidth="1"/>
-    <col min="18" max="18" width="22" customWidth="1"/>
-    <col min="19" max="19" width="51" customWidth="1"/>
-    <col min="20" max="20" width="44.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="40" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="39" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="32.1640625" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="17" max="17" width="22" customWidth="1"/>
+    <col min="18" max="18" width="51" customWidth="1"/>
+    <col min="19" max="19" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2072,1292 +2065,1281 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>444</v>
+        <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>0</v>
+        <v>445</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>445</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1</v>
+        <v>445</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>445</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>1</v>
+        <v>445</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>1</v>
+        <v>447</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>445</v>
+        <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="M2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="7">
+      <c r="G3" s="7">
         <v>43714</v>
       </c>
-      <c r="J3" s="7">
+      <c r="I3" s="7">
         <v>44271</v>
       </c>
+      <c r="R3" t="s">
+        <v>24</v>
+      </c>
       <c r="S3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D4" s="23"/>
+        <v>443</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="7">
+      <c r="G4" s="7">
         <v>38604</v>
       </c>
-      <c r="J4" s="7">
+      <c r="I4" s="7">
         <v>39348</v>
       </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
       <c r="S4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D5" s="23"/>
+        <v>443</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="7">
+      <c r="G5" s="7">
         <v>28450</v>
       </c>
-      <c r="J5" s="7">
+      <c r="I5" s="7">
         <v>31405</v>
       </c>
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
       <c r="S5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D6" s="23"/>
+        <v>443</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="7">
+      <c r="G6" s="7">
         <v>27932</v>
       </c>
-      <c r="J6" s="7">
+      <c r="I6" s="7">
         <v>29870</v>
       </c>
+      <c r="R6" t="s">
+        <v>41</v>
+      </c>
       <c r="S6" t="s">
-        <v>41</v>
-      </c>
-      <c r="T6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D7" s="23"/>
+        <v>443</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="7">
+      <c r="G7" s="7">
         <v>42752</v>
       </c>
-      <c r="J7" s="7">
+      <c r="I7" s="7">
         <v>43066</v>
       </c>
+      <c r="R7" t="s">
+        <v>46</v>
+      </c>
       <c r="S7" t="s">
-        <v>46</v>
-      </c>
-      <c r="T7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D8" s="23"/>
+        <v>443</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="7">
+      <c r="G8" s="7">
         <v>36478</v>
       </c>
-      <c r="J8" s="7">
+      <c r="I8" s="7">
         <v>38490</v>
       </c>
+      <c r="R8" t="s">
+        <v>52</v>
+      </c>
       <c r="S8" t="s">
-        <v>52</v>
-      </c>
-      <c r="T8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="7">
+      <c r="G9" s="7">
         <v>35571</v>
       </c>
-      <c r="J9" s="7">
+      <c r="I9" s="7">
         <v>39024</v>
       </c>
+      <c r="R9" t="s">
+        <v>57</v>
+      </c>
       <c r="S9" t="s">
-        <v>57</v>
-      </c>
-      <c r="T9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="7">
+      <c r="G10" s="7">
         <v>40947</v>
       </c>
-      <c r="J10" s="7">
+      <c r="I10" s="7">
         <v>42622</v>
       </c>
+      <c r="R10" t="s">
+        <v>62</v>
+      </c>
       <c r="S10" t="s">
-        <v>62</v>
-      </c>
-      <c r="T10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="7">
+      <c r="G11" s="7">
         <v>30946</v>
       </c>
-      <c r="J11" s="7">
+      <c r="I11" s="7">
         <v>33657</v>
       </c>
+      <c r="R11" t="s">
+        <v>67</v>
+      </c>
       <c r="S11" t="s">
-        <v>67</v>
-      </c>
-      <c r="T11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="7">
+      <c r="G12" s="7">
         <v>31447</v>
       </c>
-      <c r="J12" s="7">
+      <c r="I12" s="7">
         <v>32040</v>
       </c>
+      <c r="R12" t="s">
+        <v>72</v>
+      </c>
       <c r="S12" t="s">
-        <v>72</v>
-      </c>
-      <c r="T12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="7">
+      <c r="G13" s="7">
         <v>29725</v>
       </c>
-      <c r="J13" s="7">
+      <c r="I13" s="7">
         <v>31154</v>
       </c>
+      <c r="R13" t="s">
+        <v>77</v>
+      </c>
       <c r="S13" t="s">
-        <v>77</v>
-      </c>
-      <c r="T13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="7">
+      <c r="G14" s="7">
         <v>26233</v>
       </c>
-      <c r="J14" s="7">
+      <c r="I14" s="7">
         <v>28927</v>
       </c>
+      <c r="R14" t="s">
+        <v>80</v>
+      </c>
       <c r="S14" t="s">
-        <v>80</v>
-      </c>
-      <c r="T14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="7">
+      <c r="G15" s="7">
         <v>41647</v>
       </c>
-      <c r="J15" s="7">
+      <c r="I15" s="7">
         <v>44550</v>
       </c>
+      <c r="R15" t="s">
+        <v>85</v>
+      </c>
       <c r="S15" t="s">
-        <v>85</v>
-      </c>
-      <c r="T15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="7">
+      <c r="G16" s="7">
         <v>26560</v>
       </c>
-      <c r="J16" s="7">
+      <c r="I16" s="7">
         <v>30178</v>
       </c>
+      <c r="R16" t="s">
+        <v>90</v>
+      </c>
       <c r="S16" t="s">
-        <v>90</v>
-      </c>
-      <c r="T16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="7">
+      <c r="G17" s="7">
         <v>44057</v>
       </c>
-      <c r="J17" s="7">
+      <c r="I17" s="7">
         <v>47262</v>
       </c>
+      <c r="R17" t="s">
+        <v>95</v>
+      </c>
       <c r="S17" t="s">
-        <v>95</v>
-      </c>
-      <c r="T17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" t="s">
         <v>99</v>
       </c>
-      <c r="H18" s="7">
+      <c r="G18" s="7">
         <v>28307</v>
       </c>
-      <c r="J18" s="7">
+      <c r="I18" s="7">
         <v>29208</v>
       </c>
+      <c r="R18" t="s">
+        <v>100</v>
+      </c>
       <c r="S18" t="s">
-        <v>100</v>
-      </c>
-      <c r="T18" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="7">
+      <c r="G19" s="7">
         <v>26953</v>
       </c>
-      <c r="J19" s="7">
+      <c r="I19" s="7">
         <v>29676</v>
       </c>
+      <c r="R19" t="s">
+        <v>105</v>
+      </c>
       <c r="S19" t="s">
-        <v>105</v>
-      </c>
-      <c r="T19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" t="s">
         <v>109</v>
       </c>
-      <c r="H20" s="7">
+      <c r="G20" s="7">
         <v>37579</v>
       </c>
-      <c r="J20" s="7">
+      <c r="I20" s="7">
         <v>38430</v>
       </c>
+      <c r="R20" t="s">
+        <v>110</v>
+      </c>
       <c r="S20" t="s">
-        <v>110</v>
-      </c>
-      <c r="T20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="7">
+      <c r="G21" s="7">
         <v>41544</v>
       </c>
-      <c r="J21" s="7">
+      <c r="I21" s="7">
         <v>43176</v>
       </c>
+      <c r="R21" t="s">
+        <v>115</v>
+      </c>
       <c r="S21" t="s">
-        <v>115</v>
-      </c>
-      <c r="T21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D22" t="s">
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" t="s">
         <v>119</v>
       </c>
-      <c r="H22" s="7">
+      <c r="G22" s="7">
         <v>42386</v>
       </c>
-      <c r="J22" s="7">
+      <c r="I22" s="7">
         <v>43063</v>
       </c>
+      <c r="R22" t="s">
+        <v>120</v>
+      </c>
       <c r="S22" t="s">
-        <v>120</v>
-      </c>
-      <c r="T22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D23" t="s">
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" t="s">
         <v>124</v>
       </c>
-      <c r="H23" s="7">
+      <c r="G23" s="7">
         <v>38643</v>
       </c>
-      <c r="J23" s="7">
+      <c r="I23" s="7">
         <v>41570</v>
       </c>
+      <c r="R23" t="s">
+        <v>125</v>
+      </c>
       <c r="S23" t="s">
-        <v>125</v>
-      </c>
-      <c r="T23" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D24" t="s">
+        <v>127</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" t="s">
         <v>129</v>
       </c>
-      <c r="H24" s="7">
+      <c r="G24" s="7">
         <v>30434</v>
       </c>
-      <c r="J24" s="7">
+      <c r="I24" s="7">
         <v>31417</v>
       </c>
+      <c r="R24" t="s">
+        <v>130</v>
+      </c>
       <c r="S24" t="s">
-        <v>130</v>
-      </c>
-      <c r="T24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D25" t="s">
+        <v>132</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
-      </c>
-      <c r="G25" t="s">
         <v>134</v>
       </c>
-      <c r="H25" s="7">
+      <c r="G25" s="7">
         <v>41169</v>
       </c>
-      <c r="J25" s="7">
+      <c r="I25" s="7">
         <v>44348</v>
       </c>
+      <c r="R25" t="s">
+        <v>135</v>
+      </c>
       <c r="S25" t="s">
-        <v>135</v>
-      </c>
-      <c r="T25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F26" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" t="s">
         <v>139</v>
       </c>
-      <c r="H26" s="7">
+      <c r="G26" s="7">
         <v>32735</v>
       </c>
-      <c r="J26" s="7">
+      <c r="I26" s="7">
         <v>36338</v>
       </c>
+      <c r="R26" t="s">
+        <v>140</v>
+      </c>
       <c r="S26" t="s">
-        <v>140</v>
-      </c>
-      <c r="T26" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>142</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D27" t="s">
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" t="s">
         <v>145</v>
       </c>
-      <c r="H27" s="7">
+      <c r="G27" s="7">
         <v>30594</v>
       </c>
-      <c r="J27" s="7">
+      <c r="I27" s="7">
         <v>33849</v>
       </c>
+      <c r="R27" t="s">
+        <v>146</v>
+      </c>
       <c r="S27" t="s">
-        <v>146</v>
-      </c>
-      <c r="T27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>142</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D28" t="s">
+        <v>148</v>
       </c>
       <c r="E28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F28" t="s">
-        <v>149</v>
-      </c>
-      <c r="G28" t="s">
         <v>150</v>
       </c>
-      <c r="H28" s="7">
+      <c r="G28" s="7">
         <v>32358</v>
       </c>
-      <c r="J28" s="7">
+      <c r="I28" s="7">
         <v>34961</v>
       </c>
+      <c r="R28" t="s">
+        <v>151</v>
+      </c>
       <c r="S28" t="s">
-        <v>151</v>
-      </c>
-      <c r="T28" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D29" t="s">
+        <v>153</v>
       </c>
       <c r="E29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F29" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" t="s">
         <v>155</v>
       </c>
-      <c r="H29" s="7">
+      <c r="G29" s="7">
         <v>27771</v>
       </c>
-      <c r="J29" s="7">
+      <c r="I29" s="7">
         <v>30605</v>
       </c>
+      <c r="R29" t="s">
+        <v>156</v>
+      </c>
       <c r="S29" t="s">
-        <v>156</v>
-      </c>
-      <c r="T29" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D30" t="s">
+        <v>158</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" t="s">
         <v>160</v>
       </c>
-      <c r="H30" s="7">
+      <c r="G30" s="7">
         <v>36779</v>
       </c>
-      <c r="J30" s="7">
+      <c r="I30" s="7">
         <v>38512</v>
       </c>
+      <c r="R30" t="s">
+        <v>161</v>
+      </c>
       <c r="S30" t="s">
-        <v>161</v>
-      </c>
-      <c r="T30" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D31" t="s">
+        <v>163</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F31" t="s">
-        <v>164</v>
-      </c>
-      <c r="G31" t="s">
         <v>165</v>
       </c>
-      <c r="H31" s="7">
+      <c r="G31" s="7">
         <v>40745</v>
       </c>
-      <c r="J31" s="7">
+      <c r="I31" s="7">
         <v>41178</v>
       </c>
+      <c r="R31" t="s">
+        <v>166</v>
+      </c>
       <c r="S31" t="s">
-        <v>166</v>
-      </c>
-      <c r="T31" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>142</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D32" t="s">
+        <v>168</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F32" t="s">
-        <v>169</v>
-      </c>
-      <c r="G32" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="7">
+      <c r="G32" s="7">
         <v>37210</v>
       </c>
-      <c r="J32" s="7">
+      <c r="I32" s="7">
         <v>38882</v>
       </c>
+      <c r="R32" t="s">
+        <v>171</v>
+      </c>
       <c r="S32" t="s">
-        <v>171</v>
-      </c>
-      <c r="T32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>142</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D33" t="s">
+        <v>173</v>
       </c>
       <c r="E33" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F33" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" t="s">
         <v>175</v>
       </c>
-      <c r="H33" s="7">
+      <c r="G33" s="7">
         <v>26146</v>
       </c>
-      <c r="J33" s="7">
+      <c r="I33" s="7">
         <v>26462</v>
       </c>
+      <c r="R33" t="s">
+        <v>176</v>
+      </c>
       <c r="S33" t="s">
-        <v>176</v>
-      </c>
-      <c r="T33" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>142</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D34" t="s">
+        <v>178</v>
       </c>
       <c r="E34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G34" t="s">
         <v>180</v>
       </c>
-      <c r="H34" s="7">
+      <c r="G34" s="7">
         <v>36260</v>
       </c>
-      <c r="J34" s="7">
+      <c r="I34" s="7">
         <v>36694</v>
       </c>
+      <c r="R34" t="s">
+        <v>181</v>
+      </c>
       <c r="S34" t="s">
-        <v>181</v>
-      </c>
-      <c r="T34" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>142</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D35" t="s">
+        <v>183</v>
       </c>
       <c r="E35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F35" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" t="s">
         <v>185</v>
       </c>
-      <c r="H35" s="7">
+      <c r="G35" s="7">
         <v>43538</v>
       </c>
-      <c r="J35" s="7">
+      <c r="I35" s="7">
         <v>44433</v>
       </c>
+      <c r="R35" t="s">
+        <v>186</v>
+      </c>
       <c r="S35" t="s">
-        <v>186</v>
-      </c>
-      <c r="T35" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>188</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D36" t="s">
+        <v>189</v>
       </c>
       <c r="E36" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F36" t="s">
-        <v>190</v>
-      </c>
-      <c r="G36" t="s">
         <v>191</v>
       </c>
-      <c r="H36" s="7">
+      <c r="G36" s="7">
         <v>28698</v>
       </c>
-      <c r="J36" s="7">
+      <c r="I36" s="7">
         <v>31550</v>
       </c>
+      <c r="R36" t="s">
+        <v>192</v>
+      </c>
       <c r="S36" t="s">
-        <v>192</v>
-      </c>
-      <c r="T36" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>188</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D37" t="s">
+        <v>194</v>
       </c>
       <c r="E37" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F37" t="s">
-        <v>195</v>
-      </c>
-      <c r="G37" t="s">
         <v>196</v>
       </c>
-      <c r="H37" s="7">
+      <c r="G37" s="7">
         <v>29169</v>
       </c>
-      <c r="J37" s="7">
+      <c r="I37" s="7">
         <v>31091</v>
       </c>
+      <c r="R37" t="s">
+        <v>197</v>
+      </c>
       <c r="S37" t="s">
-        <v>197</v>
-      </c>
-      <c r="T37" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>188</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
+      </c>
+      <c r="D38" t="s">
+        <v>199</v>
       </c>
       <c r="E38" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F38" t="s">
-        <v>200</v>
-      </c>
-      <c r="G38" t="s">
         <v>201</v>
       </c>
-      <c r="H38" s="7">
+      <c r="G38" s="7">
         <v>30392</v>
       </c>
-      <c r="J38" s="7">
+      <c r="I38" s="7">
         <v>33481</v>
       </c>
+      <c r="R38" t="s">
+        <v>202</v>
+      </c>
       <c r="S38" t="s">
-        <v>202</v>
-      </c>
-      <c r="T38" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B39" s="6"/>
-      <c r="H39" s="8"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G39" s="8"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B40" s="6"/>
-      <c r="H40" s="8"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G40" s="8"/>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B41" s="6"/>
-      <c r="H41" s="8"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G41" s="8"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B42" s="6"/>
-      <c r="H42" s="8"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G42" s="8"/>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B43" s="6"/>
-      <c r="H43" s="8"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G43" s="8"/>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B44" s="6"/>
-      <c r="H44" s="8"/>
-      <c r="J44" s="8"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G44" s="8"/>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B45" s="6"/>
-      <c r="H45" s="8"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G45" s="8"/>
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B46" s="6"/>
-      <c r="H46" s="8"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G46" s="8"/>
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B47" s="6"/>
-      <c r="H47" s="8"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G47" s="8"/>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B48" s="6"/>
-      <c r="H48" s="8"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G48" s="8"/>
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B49" s="6"/>
-      <c r="H49" s="8"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G49" s="8"/>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B50" s="6"/>
-      <c r="H50" s="8"/>
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G50" s="8"/>
+      <c r="I50" s="8"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B51" s="6"/>
-      <c r="H51" s="8"/>
-      <c r="J51" s="8"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G51" s="8"/>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B52" s="6"/>
-      <c r="H52" s="8"/>
-      <c r="J52" s="8"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G52" s="8"/>
+      <c r="I52" s="8"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B53" s="6"/>
-      <c r="H53" s="8"/>
-      <c r="J53" s="8"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G53" s="8"/>
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B54" s="6"/>
-      <c r="H54" s="8"/>
-      <c r="J54" s="8"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G54" s="8"/>
+      <c r="I54" s="8"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B55" s="6"/>
-      <c r="H55" s="8"/>
-      <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G55" s="8"/>
+      <c r="I55" s="8"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B56" s="6"/>
-      <c r="H56" s="8"/>
-      <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G56" s="8"/>
+      <c r="I56" s="8"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B57" s="6"/>
-      <c r="H57" s="8"/>
-      <c r="J57" s="8"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G57" s="8"/>
+      <c r="I57" s="8"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B58" s="6"/>
-      <c r="H58" s="8"/>
-      <c r="J58" s="8"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G58" s="8"/>
+      <c r="I58" s="8"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B59" s="6"/>
-      <c r="H59" s="8"/>
-      <c r="J59" s="8"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G59" s="8"/>
+      <c r="I59" s="8"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B60" s="6"/>
-      <c r="H60" s="8"/>
-      <c r="J60" s="8"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G60" s="8"/>
+      <c r="I60" s="8"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B61" s="6"/>
-      <c r="H61" s="8"/>
-      <c r="J61" s="8"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G61" s="8"/>
+      <c r="I61" s="8"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B62" s="6"/>
-      <c r="H62" s="8"/>
-      <c r="J62" s="8"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="G62" s="8"/>
+      <c r="I62" s="8"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B64" s="6"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.15">
@@ -6292,23 +6274,23 @@
       <formula1>INDIRECT("RecordType")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="I3:I1038 K3:K1038" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="H3:H1038 J3:J1038" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT("DateQualifier")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N3:N1038" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="M3:M1038" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT("CopyrightStatus")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O3:O1038" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N3:N1038" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("Significance")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P3:P1038" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O3:O1038" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>INDIRECT("Boolean")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="Q3:Q1038" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P3:P1038" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>INDIRECT("SensitivityLabel")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6323,7 +6305,7 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -6405,7 +6387,7 @@
     </row>
     <row r="3" spans="1:12" ht="32" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>215</v>
@@ -6442,6 +6424,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="32" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>444</v>
+      </c>
       <c r="B4" s="14" t="s">
         <v>226</v>
       </c>

</xml_diff>

<commit_message>
No more archive files in ingests
</commit_message>
<xml_diff>
--- a/__digital_preservation_transfer.xlsx
+++ b/__digital_preservation_transfer.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="435">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
@@ -230,21 +230,6 @@
     <t xml:space="preserve">c709d6bf162ca9525559ff723d7e7b9f</t>
   </si>
   <si>
-    <t xml:space="preserve">Broken zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description for "Broken zip"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4f6776fd-ddea-4a9b-b050-de331666bc2b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corrupted files/ascii_cp437.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">276bc98079414f472b7734a1204576db</t>
-  </si>
-  <si>
     <t xml:space="preserve">Broken PDF with broken extension</t>
   </si>
   <si>
@@ -314,21 +299,6 @@
     <t xml:space="preserve">4a8c41de9aa06bc61fc2ef64f227e009</t>
   </si>
   <si>
-    <t xml:space="preserve">Broken zip file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description for "Broken zip file"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0f33f450-4394-4113-be2a-bf6541daba4b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corrupted files/révised ghislaine.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16c163cad64f2c7e4e10c2b1b84b2610</t>
-  </si>
-  <si>
     <t xml:space="preserve">Broken wav file</t>
   </si>
   <si>
@@ -357,21 +327,6 @@
   </si>
   <si>
     <t xml:space="preserve">e15bdaa90bb3b988d6f507a1cd146a60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOOM shareware version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description for "DOOM shareware version"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4e2cfb2d-f4a6-4d71-b22c-76905be87d44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">software/DoomV1.1installersw1993idSoftwareInc.action.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0b1ee491fd2003794c234f80d08b2c39</t>
   </si>
   <si>
     <t xml:space="preserve">Pretty picture – gif</t>
@@ -1806,10 +1761,10 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S41" activeCellId="0" sqref="S41"/>
+      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60.66"/>
@@ -2225,10 +2180,10 @@
         <v>71</v>
       </c>
       <c r="G12" s="8" t="n">
-        <v>30946</v>
+        <v>31447</v>
       </c>
       <c r="I12" s="8" t="n">
-        <v>33657</v>
+        <v>32040</v>
       </c>
       <c r="R12" s="0" t="s">
         <v>72</v>
@@ -2254,10 +2209,10 @@
         <v>76</v>
       </c>
       <c r="G13" s="8" t="n">
-        <v>31447</v>
+        <v>29725</v>
       </c>
       <c r="I13" s="8" t="n">
-        <v>32040</v>
+        <v>31154</v>
       </c>
       <c r="R13" s="0" t="s">
         <v>77</v>
@@ -2274,25 +2229,25 @@
         <v>25</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="G14" s="8" t="n">
+        <v>26233</v>
+      </c>
+      <c r="I14" s="8" t="n">
+        <v>28927</v>
+      </c>
+      <c r="R14" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="S14" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="G14" s="8" t="n">
-        <v>29725</v>
-      </c>
-      <c r="I14" s="8" t="n">
-        <v>31154</v>
-      </c>
-      <c r="R14" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="S14" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2303,19 +2258,19 @@
         <v>25</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>84</v>
       </c>
       <c r="G15" s="8" t="n">
-        <v>26233</v>
+        <v>41647</v>
       </c>
       <c r="I15" s="8" t="n">
-        <v>28927</v>
+        <v>44550</v>
       </c>
       <c r="R15" s="0" t="s">
         <v>85</v>
@@ -2341,10 +2296,10 @@
         <v>89</v>
       </c>
       <c r="G16" s="8" t="n">
-        <v>41647</v>
+        <v>26560</v>
       </c>
       <c r="I16" s="8" t="n">
-        <v>44550</v>
+        <v>30178</v>
       </c>
       <c r="R16" s="0" t="s">
         <v>90</v>
@@ -2370,10 +2325,10 @@
         <v>94</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>26560</v>
+        <v>28307</v>
       </c>
       <c r="I17" s="8" t="n">
-        <v>30178</v>
+        <v>29208</v>
       </c>
       <c r="R17" s="0" t="s">
         <v>95</v>
@@ -2399,10 +2354,10 @@
         <v>99</v>
       </c>
       <c r="G18" s="8" t="n">
-        <v>44057</v>
+        <v>26953</v>
       </c>
       <c r="I18" s="8" t="n">
-        <v>47262</v>
+        <v>29676</v>
       </c>
       <c r="R18" s="0" t="s">
         <v>100</v>
@@ -2428,10 +2383,10 @@
         <v>104</v>
       </c>
       <c r="G19" s="8" t="n">
-        <v>28307</v>
+        <v>41544</v>
       </c>
       <c r="I19" s="8" t="n">
-        <v>29208</v>
+        <v>43176</v>
       </c>
       <c r="R19" s="0" t="s">
         <v>105</v>
@@ -2457,10 +2412,10 @@
         <v>109</v>
       </c>
       <c r="G20" s="8" t="n">
-        <v>26953</v>
+        <v>42386</v>
       </c>
       <c r="I20" s="8" t="n">
-        <v>29676</v>
+        <v>43063</v>
       </c>
       <c r="R20" s="0" t="s">
         <v>110</v>
@@ -2486,10 +2441,10 @@
         <v>114</v>
       </c>
       <c r="G21" s="8" t="n">
-        <v>37579</v>
+        <v>38643</v>
       </c>
       <c r="I21" s="8" t="n">
-        <v>38430</v>
+        <v>41570</v>
       </c>
       <c r="R21" s="0" t="s">
         <v>115</v>
@@ -2515,10 +2470,10 @@
         <v>119</v>
       </c>
       <c r="G22" s="8" t="n">
-        <v>41544</v>
+        <v>30434</v>
       </c>
       <c r="I22" s="8" t="n">
-        <v>43176</v>
+        <v>31417</v>
       </c>
       <c r="R22" s="0" t="s">
         <v>120</v>
@@ -2544,10 +2499,10 @@
         <v>124</v>
       </c>
       <c r="G23" s="8" t="n">
-        <v>42386</v>
+        <v>41169</v>
       </c>
       <c r="I23" s="8" t="n">
-        <v>43063</v>
+        <v>44348</v>
       </c>
       <c r="R23" s="0" t="s">
         <v>125</v>
@@ -2573,10 +2528,10 @@
         <v>129</v>
       </c>
       <c r="G24" s="8" t="n">
-        <v>38643</v>
+        <v>32735</v>
       </c>
       <c r="I24" s="8" t="n">
-        <v>41570</v>
+        <v>36338</v>
       </c>
       <c r="R24" s="0" t="s">
         <v>130</v>
@@ -2602,10 +2557,10 @@
         <v>134</v>
       </c>
       <c r="G25" s="8" t="n">
-        <v>30434</v>
+        <v>30594</v>
       </c>
       <c r="I25" s="8" t="n">
-        <v>31417</v>
+        <v>33849</v>
       </c>
       <c r="R25" s="0" t="s">
         <v>135</v>
@@ -2631,10 +2586,10 @@
         <v>139</v>
       </c>
       <c r="G26" s="8" t="n">
-        <v>41169</v>
+        <v>32358</v>
       </c>
       <c r="I26" s="8" t="n">
-        <v>44348</v>
+        <v>34961</v>
       </c>
       <c r="R26" s="0" t="s">
         <v>140</v>
@@ -2660,10 +2615,10 @@
         <v>144</v>
       </c>
       <c r="G27" s="8" t="n">
-        <v>32735</v>
+        <v>27771</v>
       </c>
       <c r="I27" s="8" t="n">
-        <v>36338</v>
+        <v>30605</v>
       </c>
       <c r="R27" s="0" t="s">
         <v>145</v>
@@ -2689,10 +2644,10 @@
         <v>149</v>
       </c>
       <c r="G28" s="8" t="n">
-        <v>30594</v>
+        <v>36779</v>
       </c>
       <c r="I28" s="8" t="n">
-        <v>33849</v>
+        <v>38512</v>
       </c>
       <c r="R28" s="0" t="s">
         <v>150</v>
@@ -2718,10 +2673,10 @@
         <v>154</v>
       </c>
       <c r="G29" s="8" t="n">
-        <v>32358</v>
+        <v>40745</v>
       </c>
       <c r="I29" s="8" t="n">
-        <v>34961</v>
+        <v>41178</v>
       </c>
       <c r="R29" s="0" t="s">
         <v>155</v>
@@ -2747,10 +2702,10 @@
         <v>159</v>
       </c>
       <c r="G30" s="8" t="n">
-        <v>27771</v>
+        <v>37210</v>
       </c>
       <c r="I30" s="8" t="n">
-        <v>30605</v>
+        <v>38882</v>
       </c>
       <c r="R30" s="0" t="s">
         <v>160</v>
@@ -2776,10 +2731,10 @@
         <v>164</v>
       </c>
       <c r="G31" s="8" t="n">
-        <v>36779</v>
+        <v>26146</v>
       </c>
       <c r="I31" s="8" t="n">
-        <v>38512</v>
+        <v>26462</v>
       </c>
       <c r="R31" s="0" t="s">
         <v>165</v>
@@ -2805,10 +2760,10 @@
         <v>169</v>
       </c>
       <c r="G32" s="8" t="n">
-        <v>40745</v>
+        <v>36260</v>
       </c>
       <c r="I32" s="8" t="n">
-        <v>41178</v>
+        <v>36694</v>
       </c>
       <c r="R32" s="0" t="s">
         <v>170</v>
@@ -2834,10 +2789,10 @@
         <v>174</v>
       </c>
       <c r="G33" s="8" t="n">
-        <v>37210</v>
+        <v>43538</v>
       </c>
       <c r="I33" s="8" t="n">
-        <v>38882</v>
+        <v>44433</v>
       </c>
       <c r="R33" s="0" t="s">
         <v>175</v>
@@ -2851,28 +2806,19 @@
         <v>24</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>177</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G34" s="8" t="n">
-        <v>26146</v>
+        <v>30391</v>
       </c>
       <c r="I34" s="8" t="n">
-        <v>26462</v>
-      </c>
-      <c r="R34" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="S34" s="0" t="s">
-        <v>181</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,28 +2826,21 @@
         <v>24</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>25</v>
+        <v>178</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="D35" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="R35" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="S35" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" s="8" t="n">
-        <v>36260</v>
-      </c>
-      <c r="I35" s="8" t="n">
-        <v>36694</v>
-      </c>
-      <c r="R35" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="S35" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,28 +2848,21 @@
         <v>24</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>25</v>
+        <v>178</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="G36" s="8" t="n">
-        <v>43538</v>
-      </c>
-      <c r="I36" s="8" t="n">
-        <v>44433</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="I36" s="8"/>
       <c r="R36" s="0" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="S36" s="0" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,19 +2870,31 @@
         <v>24</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>41</v>
+        <v>25</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>189</v>
       </c>
       <c r="G37" s="8" t="n">
-        <v>30391</v>
+        <v>30392</v>
       </c>
       <c r="I37" s="8" t="n">
-        <v>44562</v>
+        <v>33481</v>
+      </c>
+      <c r="R37" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,105 +2902,44 @@
         <v>24</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="F38" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="G38" s="8" t="n">
+        <v>28450</v>
+      </c>
+      <c r="I38" s="8" t="n">
+        <v>31405</v>
+      </c>
+      <c r="R38" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="R38" s="0" t="s">
+      <c r="S38" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="S38" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="R39" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="S39" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G40" s="8" t="n">
-        <v>30392</v>
-      </c>
-      <c r="I40" s="8" t="n">
-        <v>33481</v>
-      </c>
-      <c r="R40" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="S40" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="G41" s="8" t="n">
-        <v>28450</v>
-      </c>
-      <c r="I41" s="8" t="n">
-        <v>31405</v>
-      </c>
-      <c r="R41" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="S41" s="0" t="s">
-        <v>211</v>
-      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="7"/>
+      <c r="G39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="7"/>
+      <c r="G40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="7"/>
+      <c r="G41" s="9"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="7"/>
@@ -3150,18 +3033,12 @@
     </row>
     <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="7"/>
-      <c r="G60" s="9"/>
-      <c r="I60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="7"/>
-      <c r="G61" s="9"/>
-      <c r="I61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="7"/>
-      <c r="G62" s="9"/>
-      <c r="I62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="7"/>
@@ -6082,15 +5959,9 @@
     <row r="1035" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1035" s="7"/>
     </row>
-    <row r="1036" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1036" s="7"/>
-    </row>
-    <row r="1037" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1037" s="7"/>
-    </row>
-    <row r="1038" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1038" s="7"/>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -6099,27 +5970,27 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B1038" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B1035" type="list">
       <formula1>INDIRECT("RecordType")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H3:H1038 J3:J1038" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H3:H1035 J3:J1035" type="list">
       <formula1>INDIRECT("DateQualifier")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M3:M1038" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M3:M1035" type="list">
       <formula1>INDIRECT("CopyrightStatus")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N3:N1038" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N3:N1035" type="list">
       <formula1>INDIRECT("Significance")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O3:O1038" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O3:O1035" type="list">
       <formula1>INDIRECT("Boolean")</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P3:P1038" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P3:P1035" type="list">
       <formula1>INDIRECT("SensitivityLabel")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6145,7 +6016,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.83"/>
@@ -6160,19 +6031,19 @@
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>20</v>
@@ -6184,16 +6055,16 @@
         <v>17</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6201,25 +6072,25 @@
         <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -6227,155 +6098,155 @@
         <v>25</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="0" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="0" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F7" s="15"/>
       <c r="I7" s="0" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="F8" s="15"/>
       <c r="I8" s="0" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="J8" s="19"/>
     </row>
@@ -6383,10 +6254,10 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F9" s="15"/>
       <c r="J9" s="19"/>
@@ -6395,10 +6266,10 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="17" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="F10" s="15"/>
       <c r="J10" s="19"/>
@@ -6407,10 +6278,10 @@
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="17" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="F11" s="15"/>
       <c r="J11" s="19"/>
@@ -6419,10 +6290,10 @@
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="17" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="F12" s="15"/>
     </row>
@@ -6430,10 +6301,10 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="17" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F13" s="15"/>
     </row>
@@ -6441,10 +6312,10 @@
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="17" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F14" s="15"/>
     </row>
@@ -6452,10 +6323,10 @@
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="17" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F15" s="15"/>
     </row>
@@ -6463,10 +6334,10 @@
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="17" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="F16" s="15"/>
     </row>
@@ -6474,10 +6345,10 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="17" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F17" s="15"/>
     </row>
@@ -6485,10 +6356,10 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="17" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="F18" s="15"/>
     </row>
@@ -6496,10 +6367,10 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="17" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="F19" s="15"/>
     </row>
@@ -6507,10 +6378,10 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F20" s="15"/>
     </row>
@@ -6518,10 +6389,10 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="F21" s="15"/>
     </row>
@@ -6529,10 +6400,10 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="F22" s="15"/>
     </row>
@@ -6540,10 +6411,10 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="16" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="F23" s="15"/>
     </row>
@@ -6551,10 +6422,10 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="16" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F24" s="15"/>
     </row>
@@ -6562,10 +6433,10 @@
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F25" s="15"/>
     </row>
@@ -6573,10 +6444,10 @@
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="F26" s="15"/>
     </row>
@@ -6584,10 +6455,10 @@
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="F27" s="15"/>
     </row>
@@ -6595,10 +6466,10 @@
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="16" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="F28" s="15"/>
     </row>
@@ -6606,10 +6477,10 @@
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="F29" s="15"/>
     </row>
@@ -6617,10 +6488,10 @@
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="17" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F30" s="15"/>
     </row>
@@ -6628,10 +6499,10 @@
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="17" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="F31" s="15"/>
     </row>
@@ -6639,10 +6510,10 @@
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="17" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="F32" s="15"/>
     </row>
@@ -6650,10 +6521,10 @@
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="17" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="F33" s="15"/>
     </row>
@@ -6661,10 +6532,10 @@
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="17" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="F34" s="15"/>
     </row>
@@ -6672,10 +6543,10 @@
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="17" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="F35" s="15"/>
     </row>
@@ -6683,10 +6554,10 @@
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="17" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="F36" s="15"/>
     </row>
@@ -6694,10 +6565,10 @@
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="17" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="F37" s="15"/>
     </row>
@@ -6705,10 +6576,10 @@
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="17" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="F38" s="15"/>
     </row>
@@ -6716,611 +6587,611 @@
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="17" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="F39" s="15"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="16" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="F40" s="15"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="17" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="17" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="17" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="17" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="17" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="17" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="17" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="17" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="17" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="16" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="16" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="16" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D53" s="16" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D54" s="16" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D55" s="16" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D56" s="16" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D57" s="16" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D58" s="17" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D59" s="17" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D60" s="16" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="17" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D62" s="17" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D63" s="17" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D64" s="17" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D65" s="17" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D66" s="17" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D67" s="17" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D68" s="17" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D69" s="17" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="16" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D71" s="17" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D72" s="17" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D73" s="17" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D74" s="17" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D75" s="17" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D76" s="17" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D77" s="16" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D78" s="17" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D79" s="17" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D80" s="17" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D81" s="17" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D82" s="17" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D83" s="17" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="17" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D85" s="17" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D86" s="17" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D87" s="17" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D88" s="17" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D89" s="17" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D90" s="17" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D91" s="17" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D92" s="17" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D93" s="17" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D94" s="17" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D95" s="17" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D96" s="17" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D97" s="17" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D98" s="17" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D99" s="17" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D100" s="17" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D101" s="17" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D102" s="17" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D103" s="17" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D104" s="16" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D105" s="17" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D106" s="17" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D107" s="17" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D108" s="17" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D109" s="17" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D110" s="17" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D111" s="17" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D112" s="17" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D113" s="17" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D114" s="17" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D115" s="17" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D116" s="17" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D117" s="17" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D118" s="17" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D119" s="17" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D120" s="17" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D121" s="17" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D122" s="17" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D123" s="17" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D124" s="17" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D125" s="17" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D126" s="17" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D127" s="17" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D128" s="17" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D129" s="23" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D130" s="20" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D131" s="20" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D132" s="16" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D133" s="17" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D134" s="17" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D135" s="17" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D136" s="17" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D137" s="17" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D138" s="17" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D139" s="17" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D140" s="16" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D141" s="16" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D142" s="16" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D143" s="16" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D144" s="16" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D145" s="16" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D146" s="16" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D147" s="16" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D148" s="16" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D149" s="16" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D150" s="16" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D151" s="16" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>